<commit_message>
Update files for serve God
</commit_message>
<xml_diff>
--- a/_reference_songs.xlsx
+++ b/_reference_songs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpn/Documents/walk_with_God/_work/_vec/_departments/_worship/_leader/_songs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpn/Documents/Vision_Worship_Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47900C79-19B7-C540-82B4-E46FD7F81E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E36CBCE-E733-8646-A419-93BD4671349C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>THE REFERENCE OF SONGS</t>
   </si>
@@ -447,9 +447,51 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -459,12 +501,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -475,51 +520,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -838,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" zoomScale="179" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:H33"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="179" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -865,42 +865,42 @@
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="21"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="16"/>
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="24"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="19"/>
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -924,1080 +924,1088 @@
     </row>
     <row r="5" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13" t="s">
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="17" t="s">
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="18"/>
-      <c r="N5" s="27" t="s">
+      <c r="M5" s="13"/>
+      <c r="N5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="O5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="26"/>
+      <c r="P5" s="9"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="5">
+      <c r="B6" s="6">
         <v>1</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="20"/>
+      <c r="D6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="5" t="s">
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="5" t="s">
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="M6" s="25"/>
+      <c r="M6" s="7"/>
       <c r="N6" s="4"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="25"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="7"/>
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="5">
+      <c r="B7" s="6">
         <v>2</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="20"/>
+      <c r="D7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7" t="s">
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="5" t="s">
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="M7" s="25"/>
+      <c r="M7" s="7"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="25"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="7"/>
       <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="5">
+      <c r="B8" s="6">
         <v>3</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="5" t="s">
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="5" t="s">
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="M8" s="25"/>
+      <c r="M8" s="7"/>
       <c r="N8" s="3"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="25"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="7"/>
       <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="5">
+      <c r="B9" s="6">
         <v>4</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="5" t="s">
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="5" t="s">
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="M9" s="25"/>
+      <c r="M9" s="7"/>
       <c r="N9" s="3"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="25"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="7"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="5">
+      <c r="B10" s="6">
         <v>5</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="20"/>
+      <c r="D10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="5" t="s">
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="25"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="7"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="25"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="7"/>
       <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="5">
+      <c r="B11" s="6">
         <v>6</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="15" t="s">
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="25"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="7"/>
       <c r="N11" s="3"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="25"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="7"/>
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="5">
+      <c r="B12" s="6">
         <v>7</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="5" t="s">
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="5" t="s">
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="M12" s="25"/>
+      <c r="M12" s="7"/>
       <c r="N12" s="3"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="25"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="7"/>
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="5">
+      <c r="B13" s="6">
         <v>8</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="20"/>
+      <c r="D13" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7" t="s">
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="5" t="s">
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="M13" s="25"/>
+      <c r="M13" s="7"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="25"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="7"/>
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="5">
+      <c r="B14" s="6">
         <v>9</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="20"/>
+      <c r="D14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="5" t="s">
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="28" t="s">
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="M14" s="29"/>
+      <c r="M14" s="11"/>
       <c r="N14" s="3"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="25"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="7"/>
       <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="5">
+      <c r="B15" s="6">
         <v>10</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="5" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="5" t="s">
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="28" t="s">
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="M15" s="29"/>
+      <c r="M15" s="11"/>
       <c r="N15" s="3"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="25"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="7"/>
       <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="5">
+      <c r="B16" s="6">
         <v>11</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="5" t="s">
+      <c r="C16" s="20"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="25"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="7"/>
       <c r="N16" s="3"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="25"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="7"/>
       <c r="Q16" s="1"/>
     </row>
     <row r="17" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="5">
+      <c r="B17" s="6">
         <v>12</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="5" t="s">
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="28" t="s">
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="M17" s="29"/>
+      <c r="M17" s="11"/>
       <c r="N17" s="3"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="25"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="7"/>
       <c r="Q17" s="1"/>
     </row>
     <row r="18" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="5">
+      <c r="B18" s="6">
         <v>13</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="5" t="s">
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="28" t="s">
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="M18" s="29"/>
+      <c r="M18" s="11"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="25"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="7"/>
       <c r="Q18" s="1"/>
     </row>
     <row r="19" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="5">
+      <c r="B19" s="6">
         <v>14</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="5" t="s">
+      <c r="C19" s="20"/>
+      <c r="D19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="5" t="s">
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="28" t="s">
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="M19" s="29"/>
+      <c r="M19" s="11"/>
       <c r="N19" s="3"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="25"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="7"/>
       <c r="Q19" s="1"/>
     </row>
     <row r="20" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="5">
+      <c r="B20" s="6">
         <v>15</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5" t="s">
+      <c r="C20" s="20"/>
+      <c r="D20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="5" t="s">
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="28" t="s">
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="M20" s="29"/>
+      <c r="M20" s="11"/>
       <c r="N20" s="3"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="25"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="7"/>
       <c r="Q20" s="1"/>
     </row>
     <row r="21" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="5">
+      <c r="B21" s="6">
         <v>16</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="5" t="s">
+      <c r="C21" s="20"/>
+      <c r="D21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="5" t="s">
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="28" t="s">
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="M21" s="29"/>
+      <c r="M21" s="11"/>
       <c r="N21" s="3"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="25"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="7"/>
       <c r="Q21" s="1"/>
     </row>
     <row r="22" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="5">
+      <c r="B22" s="6">
         <v>17</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="5" t="s">
+      <c r="C22" s="20"/>
+      <c r="D22" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="5" t="s">
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="28" t="s">
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="M22" s="29"/>
+      <c r="M22" s="11"/>
       <c r="N22" s="3"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="25"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="7"/>
       <c r="Q22" s="1"/>
     </row>
     <row r="23" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="5">
+      <c r="B23" s="6">
         <v>18</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="5" t="s">
+      <c r="C23" s="20"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="28" t="s">
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="M23" s="29"/>
+      <c r="M23" s="11"/>
       <c r="N23" s="3"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="25"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="7"/>
       <c r="Q23" s="1"/>
     </row>
     <row r="24" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="5">
+      <c r="B24" s="6">
         <v>19</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="5" t="s">
+      <c r="C24" s="20"/>
+      <c r="D24" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="5" t="s">
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="25"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="7"/>
       <c r="N24" s="3"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="25"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="7"/>
       <c r="Q24" s="1"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="5">
+      <c r="B25" s="6">
         <v>20</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="5" t="s">
+      <c r="C25" s="20"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="25"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="7"/>
       <c r="N25" s="3"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="25"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="7"/>
       <c r="Q25" s="1"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="B26" s="5">
+      <c r="B26" s="6">
         <v>21</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="5" t="s">
+      <c r="C26" s="20"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="25"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="7"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="25"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="7"/>
       <c r="Q26" s="1"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="5">
+      <c r="B27" s="6">
         <v>22</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="5" t="s">
+      <c r="C27" s="20"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="25"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="7"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="25"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="7"/>
       <c r="Q27" s="1"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="5">
+      <c r="B28" s="6">
         <v>23</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="5" t="s">
+      <c r="C28" s="20"/>
+      <c r="D28" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="5" t="s">
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="25"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="7"/>
       <c r="N28" s="3"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="25"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="7"/>
       <c r="Q28" s="1"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="5">
+      <c r="B29" s="6">
         <v>24</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="5" t="s">
+      <c r="C29" s="20"/>
+      <c r="D29" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="25"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="7"/>
       <c r="N29" s="3"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="25"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="7"/>
       <c r="Q29" s="1"/>
     </row>
     <row r="30" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="5">
+      <c r="B30" s="6">
         <v>25</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="5" t="s">
+      <c r="C30" s="20"/>
+      <c r="D30" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="5" t="s">
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M30" s="25"/>
+      <c r="M30" s="7"/>
       <c r="N30" s="3"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="25"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="7"/>
       <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="5">
+      <c r="B31" s="6">
         <v>26</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="5" t="s">
+      <c r="C31" s="20"/>
+      <c r="D31" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="5" t="s">
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="5" t="s">
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M31" s="25"/>
+      <c r="M31" s="7"/>
       <c r="N31" s="3"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="25"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="7"/>
       <c r="Q31" s="1"/>
     </row>
     <row r="32" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="5">
+      <c r="B32" s="6">
         <v>27</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="5" t="s">
+      <c r="C32" s="20"/>
+      <c r="D32" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="28" t="s">
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="M32" s="29"/>
+      <c r="M32" s="11"/>
       <c r="N32" s="3"/>
-      <c r="O32" s="5" t="s">
+      <c r="O32" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="P32" s="25"/>
+      <c r="P32" s="7"/>
       <c r="Q32" s="1"/>
     </row>
     <row r="33" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="5">
+      <c r="B33" s="6">
         <v>28</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="5" t="s">
+      <c r="C33" s="20"/>
+      <c r="D33" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="5" t="s">
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="25"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="M33" s="7"/>
       <c r="N33" s="3"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="25"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="7"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="5">
+      <c r="B34" s="6">
         <v>29</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="5" t="s">
+      <c r="C34" s="20"/>
+      <c r="D34" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="25"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="M34" s="11"/>
       <c r="N34" s="3"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="25"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="7"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="5">
+      <c r="B35" s="6">
         <v>30</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="5" t="s">
+      <c r="C35" s="20"/>
+      <c r="D35" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="5" t="s">
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="25"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="M35" s="11"/>
       <c r="N35" s="3"/>
-      <c r="O35" s="5"/>
-      <c r="P35" s="25"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="7"/>
       <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="5">
+      <c r="B36" s="6">
         <v>31</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="5" t="s">
+      <c r="C36" s="20"/>
+      <c r="D36" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="5" t="s">
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="25"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="M36" s="11"/>
       <c r="N36" s="3"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="25"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="7"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="5">
+      <c r="B37" s="6">
         <v>32</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="25"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="7"/>
       <c r="N37" s="3"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="25"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="7"/>
       <c r="Q37" s="1"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="B38" s="5">
+      <c r="B38" s="6">
         <v>33</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="25"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="7"/>
       <c r="N38" s="3"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="25"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="7"/>
       <c r="Q38" s="1"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
-      <c r="B39" s="5">
+      <c r="B39" s="6">
         <v>34</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="25"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="7"/>
       <c r="N39" s="3"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="25"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="7"/>
       <c r="Q39" s="1"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
-      <c r="B40" s="5">
+      <c r="B40" s="6">
         <v>35</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="25"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="7"/>
       <c r="N40" s="3"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="25"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="7"/>
       <c r="Q40" s="1"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
-      <c r="B41" s="5">
+      <c r="B41" s="6">
         <v>36</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="25"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="7"/>
       <c r="N41" s="3"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="25"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="7"/>
       <c r="Q41" s="1"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
-      <c r="B42" s="5">
+      <c r="B42" s="6">
         <v>37</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="25"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="7"/>
       <c r="N42" s="3"/>
-      <c r="O42" s="5"/>
-      <c r="P42" s="25"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="7"/>
       <c r="Q42" s="1"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="5">
+      <c r="B43" s="6">
         <v>38</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="25"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="7"/>
       <c r="N43" s="3"/>
-      <c r="O43" s="5"/>
-      <c r="P43" s="25"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="7"/>
       <c r="Q43" s="1"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
-      <c r="B44" s="5">
+      <c r="B44" s="6">
         <v>39</v>
       </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="25"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="7"/>
       <c r="N44" s="3"/>
-      <c r="O44" s="5"/>
-      <c r="P44" s="25"/>
+      <c r="O44" s="6"/>
+      <c r="P44" s="7"/>
       <c r="Q44" s="1"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
-      <c r="B45" s="5">
+      <c r="B45" s="6">
         <v>40</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="25"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="7"/>
       <c r="N45" s="3"/>
-      <c r="O45" s="5"/>
-      <c r="P45" s="25"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="7"/>
       <c r="Q45" s="1"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
-      <c r="B46" s="5">
+      <c r="B46" s="6">
         <v>41</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="25"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="7"/>
       <c r="N46" s="3"/>
-      <c r="O46" s="5"/>
-      <c r="P46" s="25"/>
+      <c r="O46" s="6"/>
+      <c r="P46" s="7"/>
       <c r="Q46" s="1"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
-      <c r="B47" s="5">
+      <c r="B47" s="6">
         <v>42</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="25"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="7"/>
       <c r="N47" s="3"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="25"/>
+      <c r="O47" s="6"/>
+      <c r="P47" s="7"/>
       <c r="Q47" s="1"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
-      <c r="B48" s="5">
+      <c r="B48" s="6">
         <v>43</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="5"/>
-      <c r="M48" s="25"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="7"/>
       <c r="N48" s="3"/>
-      <c r="O48" s="5"/>
-      <c r="P48" s="25"/>
+      <c r="O48" s="6"/>
+      <c r="P48" s="7"/>
       <c r="Q48" s="1"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
@@ -2056,43 +2064,166 @@
     </row>
   </sheetData>
   <mergeCells count="221">
-    <mergeCell ref="O48:P48"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="O43:P43"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="O45:P45"/>
-    <mergeCell ref="O46:P46"/>
-    <mergeCell ref="O47:P47"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="O37:P37"/>
-    <mergeCell ref="O38:P38"/>
-    <mergeCell ref="O39:P39"/>
-    <mergeCell ref="O40:P40"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:H12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:H15"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:H16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:H17"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:H36"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:H34"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:H40"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:H37"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:H48"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:H45"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:H46"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:H47"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:H43"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:H44"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:H42"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:H39"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="L27:M27"/>
     <mergeCell ref="L46:M46"/>
     <mergeCell ref="L47:M47"/>
     <mergeCell ref="L48:M48"/>
@@ -2117,166 +2248,43 @@
     <mergeCell ref="L39:M39"/>
     <mergeCell ref="L28:M28"/>
     <mergeCell ref="L29:M29"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:H47"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:H43"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:H44"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:H41"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:H42"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:H39"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:H48"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:H45"/>
-    <mergeCell ref="I45:K45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:H46"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:H40"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:H38"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:H36"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:H34"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:H32"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:H19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:H17"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:H15"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:H16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:H12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="O48:P48"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="O43:P43"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="O45:P45"/>
+    <mergeCell ref="O46:P46"/>
+    <mergeCell ref="O47:P47"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="O38:P38"/>
+    <mergeCell ref="O39:P39"/>
+    <mergeCell ref="O40:P40"/>
+    <mergeCell ref="O41:P41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>